<commit_message>
Power Button PSB and Code, Blean up files and Update to Neopixels
Added a PCB that acts as a intermediary to the power button allowing it
to be controlled via HTTP calls (I use it for Smartthings). The code for
the ESP  and device handler for smartthings is also included.  BOM
Updated also

Some files have been removed/renamed. and added a boot sequence to the
neopixel control code.
</commit_message>
<xml_diff>
--- a/Documentation/PCB BOMs.xlsx
+++ b/Documentation/PCB BOMs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Arcade-Project\Documentation\R2 Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Arcade-Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="125">
   <si>
     <t>Qty</t>
   </si>
@@ -326,6 +326,75 @@
   </si>
   <si>
     <t>AUX PCB BOM 12/9/2020</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>STMN</t>
+  </si>
+  <si>
+    <t>3.5MM INPUT ADAPTER PCB BOM 4/7/2021</t>
+  </si>
+  <si>
+    <t>TACT-PANA-EVQ</t>
+  </si>
+  <si>
+    <t>SDPT RELAY-JZC</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>POWERSW</t>
+  </si>
+  <si>
+    <t>Power Switch Momentart Button</t>
+  </si>
+  <si>
+    <t>2N5088</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>NPN TRANSISTOR</t>
+  </si>
+  <si>
+    <t>ESP32DEVKITC</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>ESP32 Devkit</t>
+  </si>
+  <si>
+    <t>Res 1206 330</t>
+  </si>
+  <si>
+    <t>R1,R2</t>
+  </si>
+  <si>
+    <t>1N4148</t>
+  </si>
+  <si>
+    <t>Diode 1N4148</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Red LED</t>
+  </si>
+  <si>
+    <t>PWR,WIFI</t>
+  </si>
+  <si>
+    <t>CHIPLED_1206</t>
+  </si>
+  <si>
+    <t>ST POWER PCB BOM 12/27/2021</t>
   </si>
 </sst>
 </file>
@@ -786,14 +855,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </left>
-      <right style="thin">
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -841,14 +910,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -857,6 +925,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1178,10 +1248,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,20 +1259,20 @@
     <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="41.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1359,92 +1429,92 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>1</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8" t="s">
+      <c r="A14" s="7">
+        <v>1</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8" t="s">
+      <c r="D14" s="7"/>
+      <c r="E14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <v>1</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8" t="s">
+      <c r="A15" s="7">
+        <v>1</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8" t="s">
+      <c r="D15" s="7"/>
+      <c r="E15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="7">
         <v>2</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8" t="s">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -1531,14 +1601,14 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -1752,14 +1822,14 @@
       <c r="A38" s="4"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -2076,10 +2146,367 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
+      <c r="A58" s="11"/>
+      <c r="B58" s="10"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>1</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>2</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>7</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <v>2</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
+        <v>1</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
+        <v>1</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>1</v>
+      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="11"/>
+      <c r="B68" s="10"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <v>1</v>
+      </c>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
+        <v>1</v>
+      </c>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
+        <v>1</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="3">
+        <v>1</v>
+      </c>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
+        <v>1</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
+        <v>2</v>
+      </c>
+      <c r="B76" s="3">
+        <v>330</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="3">
+        <v>1</v>
+      </c>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="3">
+        <v>2</v>
+      </c>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D78" s="3">
+        <v>1206</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
+        <v>2</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A59:F59"/>
+    <mergeCell ref="A69:F69"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A12:F12"/>
     <mergeCell ref="A18:F18"/>

</xml_diff>